<commit_message>
solver error in graph
</commit_message>
<xml_diff>
--- a/numerical_results.xlsx
+++ b/numerical_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\algar\Documents\Travail\GitHub\AIMathAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95EBDF8-D4F3-47FB-8F71-54FEAF1E7A66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD7C7E6-C3A5-49D7-B092-8ED2B8F5E09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,7 +380,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19</c:v>
@@ -1569,7 +1569,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1615,7 +1615,7 @@
         <v>20</v>
       </c>
       <c r="C4">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>